<commit_message>
updated resources as active
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-no-basis-Appointment.xlsx
+++ b/output/StructureDefinition-no-basis-Appointment.xlsx
@@ -51,7 +51,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-24T15:39:37+02:00</t>
+    <t>2023-10-04T22:15:59+02:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>